<commit_message>
excel sync for all fields
</commit_message>
<xml_diff>
--- a/project/output.xlsx
+++ b/project/output.xlsx
@@ -7,7 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Orders" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Samples" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -16,7 +17,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <name val="Calibri"/>
@@ -46,8 +49,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,6 +441,86 @@
           <t>Billing Address</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>AG and HZI</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Quote No</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Contact Phone</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Data Delivery</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Signature</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Experiment Title</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>DNA</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>RNA</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>Library</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>Method</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>Buffer</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>Organism</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>Isolated From</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>Isolation Method</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -450,6 +534,11 @@
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -463,6 +552,11 @@
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -476,38 +570,330 @@
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Order User</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Sample Name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Concentration</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Volume</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Ratio 260/280</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Ratio 260/230</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Comments</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Internal ID</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>MIxS Metadata Standard</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>MIxS Metadata</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Sample 1</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="H2" s="1" t="n">
+        <v>45390.46748519846</v>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Human Skin</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>{"project name": "a", "experimental factor": "a", "ploidy": "a", "number of replicons": "a", "extrachromosomal elements": "a", "estimated size": "a", "reference for biomaterial": "a", "annotation source": "a", "sample volume or weight for DNA extraction": "a", "nucleic acid extraction": "", "nucleic acid amplification": "a", "library size": "a", "library reads sequenced": "a", "library construction method": "a", "library vector": "a", "library screening strategy": "a", "target gene": "a", "target subfragment": "a", "pcr primers": "a", "multiplex identifiers": "a", "adapters": "a", "pcr conditions": "", "sequencing method": "aa", "chimera check software": "", "relevant electronic resources": "a", "relevant standard operating procedures": "a", "negative control type": "a", "positive control type": "a", "collection date": "a", "geographic location (latitude)": "", "geographic location (longitude)": "", "geographic location (region and locality)": "", "broad-scale environmental context": "", "local environmental context": "", "environmental medium": "", "source material identifiers": "", "sample material processing": "", "isolation and growth condition": "", "propagation": "", "amount or size of sample collected": "", "host body product": "", "organism count": "", "sample storage duration": "", "sample storage temperature": "", "sample storage location": "", "sample collection device": "", "sample collection method": "", "host disease status": "", "lung/pulmonary disorder": "", "lung/nose-throat disorder": "", "blood/blood disorder": "", "urine/kidney disorder": "", "urine/urogenital tract disorder": "", "host subject id": "", "host age": "", "host body site": "", "drug usage": "", "host height": "", "host body-mass index": "", "ethnicity": "", "host total mass": "", "host phenotype": "", "host body temperature": "", "host scientific name": "", "presence of pets or farm animals": "", "temperature": "", "salinity": "", "major diet change in last six months": "", "weight loss in last three months": "", "travel outside the country in last six months": "", "host diet": "", "twin sibling presence": "", "host last meal": "", "amniotic fluid/gestation state": "", "host family relationship": "", "amniotic fluid/maternal health status": "", "host genotype": "", "amniotic fluid/foetal health status": "", "host pulse": "", "amniotic fluid/color": "", "subspecific genetic lineage": "", "known pathogenicity": "", "encoded traits": "", "chemical administration": "", "perturbation": ""}</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Sample 2</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="H3" s="1" t="n">
+        <v>45390.46748522203</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Human Associated</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>{"project name": "b", "experimental factor": "b", "ploidy": "b", "number of replicons": "b", "extrachromosomal elements": "b", "estimated size": "", "reference for biomaterial": "", "annotation source": "", "sample volume or weight for DNA extraction": "", "nucleic acid extraction": "", "nucleic acid amplification": "", "library size": "", "library reads sequenced": "", "library construction method": "", "library vector": "", "library screening strategy": "", "target gene": "", "target subfragment": "", "pcr primers": "", "multiplex identifiers": "", "adapters": "", "pcr conditions": "", "sequencing method": "", "chimera check software": "", "relevant electronic resources": "", "relevant standard operating procedures": "", "negative control type": "", "positive control type": "", "collection date": "", "geographic location (latitude)": "", "geographic location (longitude)": "", "geographic location (region and locality)": "", "broad-scale environmental context": "", "local environmental context": "", "environmental medium": "", "source material identifiers": "", "sample material processing": "", "isolation and growth condition": "", "propagation": "", "amount or size of sample collected": "", "host body product": "", "organism count": "", "sample storage duration": "", "sample storage temperature": "", "sample storage location": "", "sample collection device": "", "sample collection method": "", "host disease status": "", "lung/pulmonary disorder": "", "lung/nose-throat disorder": "", "blood/blood disorder": "", "urine/kidney disorder": "", "urine/urogenital tract disorder": "", "host subject id": "", "host age": "", "host body site": "", "drug usage": "", "host height": "", "host body-mass index": "", "ethnicity": "", "host total mass": "", "host phenotype": "", "host body temperature": "", "host scientific name": "", "presence of pets or farm animals": "", "temperature": "", "salinity": "", "major diet change in last six months": "", "weight loss in last three months": "", "travel outside the country in last six months": "", "host diet": "", "twin sibling presence": "", "host last meal": "", "amniotic fluid/gestation state": "", "host family relationship": "", "amniotic fluid/maternal health status": "", "host genotype": "", "amniotic fluid/foetal health status": "", "host pulse": "", "amniotic fluid/color": "", "subspecific genetic lineage": "", "known pathogenicity": "", "encoded traits": "", "chemical administration": "", "perturbation": ""}</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>test1</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Sample 1</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="H4" s="1" t="n">
+        <v>45390.47341535308</v>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Air</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>{"cell_type": "a", "dev_stage": null, "germline": null, "tissue_lib": null, "tissue_type": null, "isolation_source": null, "lat_lon": null, "collection date": null, "geographic location (region and locality)": null, "identified_by": null, "mating_type": null, "sex": null, "lab_host": null, "host scientific name": null, "bio_material": null, "culture_collection": null, "specimen_voucher": null, "cultivar": null, "ecotype": null, "isolate": null, "sub_species": null, "variety": null, "sub_strain": null, "cell_line": null, "serotype": null, "serovar": null, "strain": null}</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>test1</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Sample 1</t>
+          <t>Sample 2</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="H5" s="1" t="n">
+        <v>45390.4734153825</v>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Air</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>{"cell_type": "a", "dev_stage": null, "germline": null, "tissue_lib": null, "tissue_type": null, "isolation_source": null, "lat_lon": null, "collection date": null, "geographic location (region and locality)": null, "identified_by": null, "mating_type": null, "sex": null, "lab_host": null, "host scientific name": null, "bio_material": null, "culture_collection": null, "specimen_voucher": null, "cultivar": null, "ecotype": null, "isolate": null, "sub_species": null, "variety": null, "sub_strain": null, "cell_line": null, "serotype": null, "serovar": null, "strain": null}</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>test1</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Sample 2</t>
+          <t>Sample 3</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>b</t>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="H6" s="1" t="n">
+        <v>45390.47341540964</v>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Soil</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>{"slope gradient": "b", "slope aspect": null, "project name": null, "experimental factor": null, "ploidy": null, "number of replicons": null, "extrachromosomal elements": null, "estimated size": null, "reference for biomaterial": null, "annotation source": null, "sample volume or weight for DNA extraction": null, "nucleic acid extraction": null, "nucleic acid amplification": null, "library size": null, "library reads sequenced": null, "library construction method": null, "library vector": null, "library screening strategy": null, "target gene": null, "target subfragment": null, "pcr primers": null, "multiplex identifiers": null, "adapters": null, "pcr conditions": null, "sequencing method": null, "chimera check software": null, "relevant electronic resources": null, "relevant standard operating procedures": null, "pooling of DNA extracts (if done)": null, "negative control type": null, "positive control type": null, "collection date": null, "altitude": null, "geographic location (latitude)": null, "geographic location (longitude)": null, "geographic location (region and locality)": null, "depth": null, "broad-scale environmental context": null, "local environmental context": null, "environmental medium": null, "elevation": null, "source material identifiers": null, "sample material processing": null, "isolation and growth condition": null, "propagation": null, "amount or size of sample collected": null, "composite design/sieving (if any)": null, "sample weight for DNA extraction": null, "storage conditions (fresh/frozen/other)": null, "microbial biomass": null, "microbial biomass method": null, "sample collection device": null, "sample collection method": null, "salinity method": null, "extreme_unusual_properties/heavy metals": null, "extreme_unusual_properties/heavy metals method": null, "extreme_unusual_properties/Al saturation": null, "extreme_unusual_properties/Al saturation method": null, "host disease status": null, "host scientific name": null, "link to climate information": null, "link to classification information": null, "links to additional analysis": null, "current land use": null, "current vegetation": null, "current vegetation method": null, "soil horizon method": null, "mean annual and seasonal temperature": null, "mean annual and seasonal precipitation": null, "soil_taxonomic/FAO classification": null, "soil_taxonomic/local classification": null, "soil_taxonomic/local classification method": null, "soil type method": null, "temperature": null, "soil texture measurement": null, "soil texture method": null, "pH": null, "pH method": null, "water content method": null, "total organic C method": null, "total nitrogen method": null, "organic matter": null, "total organic carbon": null, "water content": null, "total nitrogen": null, "history/previous land use": null, "history/previous land use method": null, "history/crop rotation": null, "history/agrochemical additions": null, "history/fire": null, "history/flooding": null, "history/extreme events": null, "subspecific genetic lineage": null, "known pathogenicity": null, "encoded traits": null, "perturbation": null}</t>
         </is>
       </c>
     </row>
@@ -519,12 +905,45 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Sample 1</t>
+          <t>Sample 4</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="H7" s="1" t="n">
+        <v>45390.47341543507</v>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Air</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>{"cell_type": "a", "dev_stage": null, "germline": null, "tissue_lib": null, "tissue_type": null, "isolation_source": null, "lat_lon": null, "collection date": null, "geographic location (region and locality)": null, "identified_by": null, "mating_type": null, "sex": null, "lab_host": null, "host scientific name": null, "bio_material": null, "culture_collection": null, "specimen_voucher": null, "cultivar": null, "ecotype": null, "isolate": null, "sub_species": null, "variety": null, "sub_strain": null, "cell_line": null, "serotype": null, "serovar": null, "strain": null}</t>
         </is>
       </c>
     </row>
@@ -536,12 +955,45 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Sample 2</t>
+          <t>Sample 1</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>b</t>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="H8" s="1" t="n">
+        <v>45390.4737031342</v>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Air</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>{"project name": "aa", "experimental factor": "a", "ploidy": "a", "number of replicons": null, "extrachromosomal elements": null, "estimated size": null, "reference for biomaterial": null, "annotation source": null, "sample volume or weight for DNA extraction": null, "nucleic acid extraction": null, "nucleic acid amplification": null, "library size": null, "library reads sequenced": null, "library construction method": null, "library vector": null, "library screening strategy": null, "target gene": null, "target subfragment": null, "pcr primers": null, "multiplex identifiers": null, "adapters": null, "pcr conditions": null, "sequencing method": null, "chimera check software": null, "relevant electronic resources": null, "relevant standard operating procedures": null, "negative control type": null, "positive control type": null, "collection date": null, "altitude": null, "geographic location (latitude)": null, "geographic location (longitude)": null, "geographic location (region and locality)": null, "depth": null, "broad-scale environmental context": null, "local environmental context": null, "environmental medium": null, "elevation": null, "source material identifiers": null, "sample material processing": null, "isolation and growth condition": null, "propagation": null, "amount or size of sample collected": null, "host body product": null, "host dry mass": null, "organism count": null, "sample storage duration": null, "sample storage temperature": null, "sample storage location": null, "host disease status": null, "host common name": null, "host subject id": null, "host age": null, "host taxid": null, "host body habitat": null, "host body site": null, "host life stage": null, "host height": null, "host length": null, "host growth conditions": null, "host substrate": null, "host total mass": null, "host phenotype": null, "host body temperature": null, "host color": null, "host shape": null, "host scientific name": null, "host subspecific genetic lineage": null, "temperature": null, "salinity": null, "host blood pressure diastolic": null, "host blood pressure systolic": null, "host diet": null, "host last meal": null, "host family relationship": null, "host genotype": null, "gravidity": null, "subspecific genetic lineage": null, "known pathogenicity": null, "encoded traits": null, "chemical administration": null, "perturbation": null}</t>
         </is>
       </c>
     </row>
@@ -553,12 +1005,45 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Sample 3</t>
+          <t>Sample 2</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>c</t>
+          <t>aa</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="H9" s="1" t="n">
+        <v>45390.47370316552</v>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Soil</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>{"project name": null, "experimental factor": null, "ploidy": null, "number of replicons": null, "extrachromosomal elements": null, "estimated size": null, "reference for biomaterial": null, "annotation source": null, "sample volume or weight for DNA extraction": null, "nucleic acid extraction": null, "nucleic acid amplification": null, "library size": null, "library reads sequenced": null, "library construction method": null, "library vector": null, "library screening strategy": null, "target gene": null, "target subfragment": null, "pcr primers": null, "multiplex identifiers": null, "adapters": null, "pcr conditions": null, "sequencing method": null, "chimera check software": null, "relevant electronic resources": null, "relevant standard operating procedures": null, "negative control type": null, "positive control type": null, "collection date": null, "altitude": null, "geographic location (latitude)": null, "geographic location (longitude)": null, "geographic location (region and locality)": null, "depth": null, "broad-scale environmental context": null, "local environmental context": null, "environmental medium": null, "elevation": null, "source material identifiers": null, "sample material processing": null, "isolation and growth condition": null, "propagation": null, "amount or size of sample collected": null, "host body product": null, "host dry mass": null, "organism count": null, "sample storage duration": null, "sample storage temperature": null, "sample storage location": null, "host disease status": null, "host common name": null, "host subject id": null, "host age": null, "host taxid": null, "host body habitat": null, "host body site": null, "host life stage": null, "host height": null, "host length": null, "host growth conditions": null, "host substrate": null, "host total mass": null, "host phenotype": null, "host body temperature": null, "host color": null, "host shape": null, "host scientific name": null, "host subspecific genetic lineage": null, "temperature": null, "salinity": null, "host blood pressure diastolic": null, "host blood pressure systolic": null, "host diet": null, "host last meal": null, "host family relationship": null, "host genotype": null, "gravidity": null, "subspecific genetic lineage": null, "known pathogenicity": null, "encoded traits": null, "chemical administration": null, "perturbation": null}</t>
         </is>
       </c>
     </row>
@@ -570,63 +1055,45 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Sample 4</t>
+          <t>Sample 3</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>d</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>test1</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Sample 1</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>test1</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Sample 2</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
           <t>aa</t>
         </is>
       </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>test1</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Sample 3</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>aa</t>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>aaa</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="H10" s="1" t="n">
+        <v>45390.47370319343</v>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Host Associated</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>{"project name": null, "experimental factor": null, "ploidy": null, "number of replicons": null, "extrachromosomal elements": null, "estimated size": null, "reference for biomaterial": null, "annotation source": null, "sample volume or weight for DNA extraction": null, "nucleic acid extraction": null, "nucleic acid amplification": null, "library size": null, "library reads sequenced": null, "library construction method": null, "library vector": null, "library screening strategy": null, "target gene": null, "target subfragment": null, "pcr primers": null, "multiplex identifiers": null, "adapters": null, "pcr conditions": null, "sequencing method": null, "chimera check software": null, "relevant electronic resources": null, "relevant standard operating procedures": null, "negative control type": null, "positive control type": null, "collection date": null, "altitude": null, "geographic location (latitude)": null, "geographic location (longitude)": null, "geographic location (region and locality)": null, "depth": null, "broad-scale environmental context": null, "local environmental context": null, "environmental medium": null, "elevation": null, "source material identifiers": null, "sample material processing": null, "isolation and growth condition": null, "propagation": null, "amount or size of sample collected": null, "host body product": null, "host dry mass": null, "organism count": null, "sample storage duration": null, "sample storage temperature": null, "sample storage location": null, "host disease status": null, "host common name": null, "host subject id": null, "host age": null, "host taxid": null, "host body habitat": null, "host body site": null, "host life stage": null, "host height": null, "host length": null, "host growth conditions": null, "host substrate": null, "host total mass": null, "host phenotype": null, "host body temperature": null, "host color": null, "host shape": null, "host scientific name": null, "host subspecific genetic lineage": null, "temperature": null, "salinity": null, "host blood pressure diastolic": null, "host blood pressure systolic": null, "host diet": null, "host last meal": null, "host family relationship": null, "host genotype": null, "gravidity": null, "subspecific genetic lineage": null, "known pathogenicity": null, "encoded traits": null, "chemical administration": null, "perturbation": null}</t>
         </is>
       </c>
     </row>

</xml_diff>